<commit_message>
1. change lab test result field from testresult to testresult_calc
</commit_message>
<xml_diff>
--- a/CPCSSNReport/DataTemplate.xlsx
+++ b/CPCSSNReport/DataTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="86">
   <si>
     <t>Males</t>
   </si>
@@ -260,13 +260,25 @@
   </si>
   <si>
     <t>LABA</t>
+  </si>
+  <si>
+    <t>Epilepsy</t>
+  </si>
+  <si>
+    <t>Dementia</t>
+  </si>
+  <si>
+    <t>Parkinson's Disease</t>
+  </si>
+  <si>
+    <t>0-17 years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -413,6 +425,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,6 +438,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -498,6 +521,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -532,6 +556,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -707,19 +732,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX10" sqref="AX10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="26.25" thickBot="1">
+    <row r="1" spans="1:68" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -746,8 +772,17 @@
       <c r="AL1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:44" ht="15.75" thickBot="1">
+      <c r="AT1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -849,8 +884,65 @@
       <c r="AR2" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:44" ht="30.75" thickBot="1">
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AY2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ2" s="5"/>
+      <c r="BK2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BM2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="BO2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP2" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:68" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -858,7 +950,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="F3" s="7" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -867,7 +959,7 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="N3" s="7" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
@@ -876,7 +968,7 @@
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="V3" s="7" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
@@ -885,7 +977,7 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
       <c r="AD3" s="7" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="AE3" s="8"/>
       <c r="AF3" s="8"/>
@@ -894,7 +986,7 @@
       <c r="AI3" s="8"/>
       <c r="AJ3" s="8"/>
       <c r="AL3" s="7" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="AM3" s="8"/>
       <c r="AN3" s="8"/>
@@ -902,8 +994,35 @@
       <c r="AP3" s="8"/>
       <c r="AQ3" s="8"/>
       <c r="AR3" s="8"/>
-    </row>
-    <row r="4" spans="1:44" ht="30.75" thickBot="1">
+      <c r="AT3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BB3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="BC3" s="8"/>
+      <c r="BD3" s="8"/>
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="8"/>
+      <c r="BG3" s="8"/>
+      <c r="BH3" s="8"/>
+      <c r="BJ3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="BK3" s="8"/>
+      <c r="BL3" s="8"/>
+      <c r="BM3" s="8"/>
+      <c r="BN3" s="8"/>
+      <c r="BO3" s="8"/>
+      <c r="BP3" s="8"/>
+    </row>
+    <row r="4" spans="1:68" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -911,7 +1030,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="F4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -920,7 +1039,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="N4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
@@ -929,7 +1048,7 @@
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
       <c r="V4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
@@ -938,7 +1057,7 @@
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
       <c r="AD4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE4" s="8"/>
       <c r="AF4" s="8"/>
@@ -947,7 +1066,7 @@
       <c r="AI4" s="8"/>
       <c r="AJ4" s="8"/>
       <c r="AL4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AM4" s="8"/>
       <c r="AN4" s="8"/>
@@ -955,8 +1074,35 @@
       <c r="AP4" s="8"/>
       <c r="AQ4" s="8"/>
       <c r="AR4" s="8"/>
-    </row>
-    <row r="5" spans="1:44" ht="30.75" thickBot="1">
+      <c r="AT4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BB4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="BC4" s="8"/>
+      <c r="BD4" s="8"/>
+      <c r="BE4" s="8"/>
+      <c r="BF4" s="8"/>
+      <c r="BG4" s="8"/>
+      <c r="BH4" s="8"/>
+      <c r="BJ4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="BK4" s="8"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8"/>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="8"/>
+    </row>
+    <row r="5" spans="1:68" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -964,7 +1110,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="F5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -973,7 +1119,7 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="N5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
@@ -982,7 +1128,7 @@
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
       <c r="V5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
@@ -991,7 +1137,7 @@
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
       <c r="AD5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE5" s="8"/>
       <c r="AF5" s="8"/>
@@ -1000,7 +1146,7 @@
       <c r="AI5" s="8"/>
       <c r="AJ5" s="8"/>
       <c r="AL5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AM5" s="8"/>
       <c r="AN5" s="8"/>
@@ -1008,8 +1154,35 @@
       <c r="AP5" s="8"/>
       <c r="AQ5" s="8"/>
       <c r="AR5" s="8"/>
-    </row>
-    <row r="6" spans="1:44" ht="30.75" thickBot="1">
+      <c r="AT5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU5" s="8"/>
+      <c r="AV5" s="8"/>
+      <c r="AW5" s="8"/>
+      <c r="AX5" s="8"/>
+      <c r="AY5" s="8"/>
+      <c r="AZ5" s="8"/>
+      <c r="BB5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BC5" s="8"/>
+      <c r="BD5" s="8"/>
+      <c r="BE5" s="8"/>
+      <c r="BF5" s="8"/>
+      <c r="BG5" s="8"/>
+      <c r="BH5" s="8"/>
+      <c r="BJ5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="BK5" s="8"/>
+      <c r="BL5" s="8"/>
+      <c r="BM5" s="8"/>
+      <c r="BN5" s="8"/>
+      <c r="BO5" s="8"/>
+      <c r="BP5" s="8"/>
+    </row>
+    <row r="6" spans="1:68" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1017,7 +1190,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="F6" s="7" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -1026,7 +1199,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="N6" s="7" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -1035,7 +1208,7 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
       <c r="V6" s="7" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
@@ -1044,7 +1217,7 @@
       <c r="AA6" s="8"/>
       <c r="AB6" s="8"/>
       <c r="AD6" s="7" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="AE6" s="8"/>
       <c r="AF6" s="8"/>
@@ -1053,7 +1226,7 @@
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8"/>
       <c r="AL6" s="7" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="AM6" s="8"/>
       <c r="AN6" s="8"/>
@@ -1061,8 +1234,35 @@
       <c r="AP6" s="8"/>
       <c r="AQ6" s="8"/>
       <c r="AR6" s="8"/>
-    </row>
-    <row r="7" spans="1:44" ht="15.75" thickBot="1">
+      <c r="AT6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="8"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+      <c r="BB6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BC6" s="8"/>
+      <c r="BD6" s="8"/>
+      <c r="BE6" s="8"/>
+      <c r="BF6" s="8"/>
+      <c r="BG6" s="8"/>
+      <c r="BH6" s="8"/>
+      <c r="BJ6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK6" s="8"/>
+      <c r="BL6" s="8"/>
+      <c r="BM6" s="8"/>
+      <c r="BN6" s="8"/>
+      <c r="BO6" s="8"/>
+      <c r="BP6" s="8"/>
+    </row>
+    <row r="7" spans="1:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1070,7 +1270,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="F7" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -1079,7 +1279,7 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="N7" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -1088,7 +1288,7 @@
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
       <c r="V7" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="W7" s="8"/>
       <c r="X7" s="8"/>
@@ -1097,7 +1297,7 @@
       <c r="AA7" s="8"/>
       <c r="AB7" s="8"/>
       <c r="AD7" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
@@ -1106,7 +1306,7 @@
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8"/>
       <c r="AL7" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="AM7" s="8"/>
       <c r="AN7" s="8"/>
@@ -1114,113 +1314,116 @@
       <c r="AP7" s="8"/>
       <c r="AQ7" s="8"/>
       <c r="AR7" s="8"/>
-    </row>
-    <row r="8" spans="1:44" ht="15.75" thickBot="1">
+      <c r="AT7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU7" s="8"/>
+      <c r="AV7" s="8"/>
+      <c r="AW7" s="8"/>
+      <c r="AX7" s="8"/>
+      <c r="AY7" s="8"/>
+      <c r="AZ7" s="8"/>
+      <c r="BB7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC7" s="8"/>
+      <c r="BD7" s="8"/>
+      <c r="BE7" s="8"/>
+      <c r="BF7" s="8"/>
+      <c r="BG7" s="8"/>
+      <c r="BH7" s="8"/>
+      <c r="BJ7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="BK7" s="8"/>
+      <c r="BL7" s="8"/>
+      <c r="BM7" s="8"/>
+      <c r="BN7" s="8"/>
+      <c r="BO7" s="8"/>
+      <c r="BP7" s="8"/>
+    </row>
+    <row r="8" spans="1:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:44" ht="15.75" thickBot="1">
-      <c r="F9" s="5"/>
-      <c r="G9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="V9" s="5"/>
-      <c r="W9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL9" s="5"/>
-      <c r="AM9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AR9" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" ht="60.75" thickBot="1">
+      <c r="F8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="N8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="V8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AD8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AL8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM8" s="8"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="8"/>
+      <c r="AR8" s="8"/>
+      <c r="AT8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="8"/>
+      <c r="AW8" s="8"/>
+      <c r="AX8" s="8"/>
+      <c r="AY8" s="8"/>
+      <c r="AZ8" s="8"/>
+      <c r="BB8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC8" s="8"/>
+      <c r="BD8" s="8"/>
+      <c r="BE8" s="8"/>
+      <c r="BF8" s="8"/>
+      <c r="BG8" s="8"/>
+      <c r="BH8" s="8"/>
+      <c r="BJ8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK8" s="8"/>
+      <c r="BL8" s="8"/>
+      <c r="BM8" s="8"/>
+      <c r="BN8" s="8"/>
+      <c r="BO8" s="8"/>
+      <c r="BP8" s="8"/>
+    </row>
+    <row r="9" spans="1:68" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:68" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -1228,60 +1431,110 @@
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="N10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="V10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
-      <c r="AD10" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="8"/>
-      <c r="AH10" s="8"/>
-      <c r="AI10" s="8"/>
-      <c r="AJ10" s="8"/>
-      <c r="AL10" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM10" s="8"/>
-      <c r="AN10" s="8"/>
-      <c r="AO10" s="8"/>
-      <c r="AP10" s="8"/>
-      <c r="AQ10" s="8"/>
-      <c r="AR10" s="8"/>
-    </row>
-    <row r="11" spans="1:44" ht="26.25" thickBot="1">
+      <c r="F10" s="5"/>
+      <c r="G10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="V10" s="5"/>
+      <c r="W10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR10" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:68" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="F11" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1290,7 +1543,7 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="N11" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
@@ -1299,7 +1552,7 @@
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
       <c r="V11" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W11" s="8"/>
       <c r="X11" s="8"/>
@@ -1308,7 +1561,7 @@
       <c r="AA11" s="8"/>
       <c r="AB11" s="8"/>
       <c r="AD11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AE11" s="8"/>
       <c r="AF11" s="8"/>
@@ -1317,7 +1570,7 @@
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8"/>
       <c r="AL11" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AM11" s="8"/>
       <c r="AN11" s="8"/>
@@ -1326,14 +1579,14 @@
       <c r="AQ11" s="8"/>
       <c r="AR11" s="8"/>
     </row>
-    <row r="12" spans="1:44" ht="51.75" thickBot="1">
+    <row r="12" spans="1:68" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="F12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1342,7 +1595,7 @@
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
       <c r="N12" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
@@ -1351,7 +1604,7 @@
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
       <c r="V12" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
@@ -1360,7 +1613,7 @@
       <c r="AA12" s="8"/>
       <c r="AB12" s="8"/>
       <c r="AD12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AE12" s="8"/>
       <c r="AF12" s="8"/>
@@ -1369,7 +1622,7 @@
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8"/>
       <c r="AL12" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM12" s="8"/>
       <c r="AN12" s="8"/>
@@ -1378,14 +1631,14 @@
       <c r="AQ12" s="8"/>
       <c r="AR12" s="8"/>
     </row>
-    <row r="13" spans="1:44" ht="26.25" thickBot="1">
+    <row r="13" spans="1:68" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="F13" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1394,7 +1647,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="N13" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
@@ -1403,7 +1656,7 @@
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
       <c r="V13" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W13" s="8"/>
       <c r="X13" s="8"/>
@@ -1412,7 +1665,7 @@
       <c r="AA13" s="8"/>
       <c r="AB13" s="8"/>
       <c r="AD13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE13" s="8"/>
       <c r="AF13" s="8"/>
@@ -1421,7 +1674,7 @@
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8"/>
       <c r="AL13" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AM13" s="8"/>
       <c r="AN13" s="8"/>
@@ -1430,14 +1683,14 @@
       <c r="AQ13" s="8"/>
       <c r="AR13" s="8"/>
     </row>
-    <row r="14" spans="1:44" ht="51.75" thickBot="1">
+    <row r="14" spans="1:68" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="F14" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -1446,7 +1699,7 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="N14" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
@@ -1455,7 +1708,7 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
       <c r="V14" s="7" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="W14" s="8"/>
       <c r="X14" s="8"/>
@@ -1464,22 +1717,16 @@
       <c r="AA14" s="8"/>
       <c r="AB14" s="8"/>
       <c r="AD14" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE14" s="8" t="s">
-        <v>26</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="AE14" s="8"/>
       <c r="AF14" s="8"/>
-      <c r="AG14" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="AG14" s="8"/>
       <c r="AH14" s="8"/>
-      <c r="AI14" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="AI14" s="8"/>
       <c r="AJ14" s="8"/>
       <c r="AL14" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AM14" s="8"/>
       <c r="AN14" s="8"/>
@@ -1488,14 +1735,14 @@
       <c r="AQ14" s="8"/>
       <c r="AR14" s="8"/>
     </row>
-    <row r="15" spans="1:44" ht="39" thickBot="1">
+    <row r="15" spans="1:68" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="F15" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1504,7 +1751,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="N15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
@@ -1512,8 +1759,17 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
+      <c r="V15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
       <c r="AD15" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE15" s="8" t="s">
         <v>26</v>
@@ -1527,10 +1783,24 @@
         <v>26</v>
       </c>
       <c r="AJ15" s="8"/>
-    </row>
-    <row r="16" spans="1:44" ht="15.75" thickBot="1">
+      <c r="AL15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AM15" s="8"/>
+      <c r="AN15" s="8"/>
+      <c r="AO15" s="8"/>
+      <c r="AP15" s="8"/>
+      <c r="AQ15" s="8"/>
+      <c r="AR15" s="8"/>
+    </row>
+    <row r="16" spans="1:68" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
       <c r="F16" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -1538,93 +1808,93 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="V16" s="9"/>
-      <c r="W16" s="10" t="s">
+      <c r="N16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="AD16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ16" s="8"/>
+    </row>
+    <row r="17" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="F17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="X16" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y16" s="10" t="s">
+      <c r="X17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="Z16" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA16" s="10" t="s">
+      <c r="Z17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AB16" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="6:28" ht="26.25" thickBot="1">
-      <c r="N17" s="5"/>
-      <c r="O17" s="6" t="s">
+      <c r="AB17" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q17" s="6" t="s">
+      <c r="P18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="R17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="S17" s="6" t="s">
+      <c r="R18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="S18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="V17" s="7" t="s">
+      <c r="T18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="V18" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="W17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB17" s="11"/>
-    </row>
-    <row r="18" spans="6:28" ht="26.25" thickBot="1">
-      <c r="F18" s="9"/>
-      <c r="G18" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L18" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="V18" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="W18" s="11" t="s">
         <v>26</v>
@@ -1639,24 +1909,28 @@
       </c>
       <c r="AB18" s="11"/>
     </row>
-    <row r="19" spans="6:28" ht="77.25" thickBot="1">
-      <c r="F19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="L19" s="11"/>
+    <row r="19" spans="1:28" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="9"/>
+      <c r="G19" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="N19" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
@@ -1665,27 +1939,39 @@
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
       <c r="V19" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
-    </row>
-    <row r="20" spans="6:28" ht="64.5" thickBot="1">
+        <v>60</v>
+      </c>
+      <c r="W19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB19" s="11"/>
+    </row>
+    <row r="20" spans="1:28" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="I20" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="K20" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="L20" s="11"/>
       <c r="N20" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
@@ -1694,24 +1980,18 @@
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
       <c r="V20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="W20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB20" s="11"/>
-    </row>
-    <row r="21" spans="6:28" ht="51.75" thickBot="1">
+        <v>61</v>
+      </c>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+    </row>
+    <row r="21" spans="1:28" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F21" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -1720,7 +2000,7 @@
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
       <c r="N21" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
@@ -1729,7 +2009,7 @@
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
       <c r="V21" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W21" s="11" t="s">
         <v>26</v>
@@ -1744,9 +2024,9 @@
       </c>
       <c r="AB21" s="11"/>
     </row>
-    <row r="22" spans="6:28" ht="39" thickBot="1">
+    <row r="22" spans="1:28" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -1755,7 +2035,7 @@
       <c r="K22" s="11"/>
       <c r="L22" s="11"/>
       <c r="N22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
@@ -1763,25 +2043,34 @@
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
-    </row>
-    <row r="23" spans="6:28" ht="51.75" thickBot="1">
+      <c r="V22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB22" s="11"/>
+    </row>
+    <row r="23" spans="1:28" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F23" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>26</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G23" s="11"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="I23" s="11"/>
       <c r="J23" s="11"/>
-      <c r="K23" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="K23" s="11"/>
       <c r="L23" s="11"/>
       <c r="N23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
@@ -1789,19 +2078,10 @@
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
-      <c r="V23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
-    </row>
-    <row r="24" spans="6:28" ht="39" thickBot="1">
+    </row>
+    <row r="24" spans="1:28" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>26</v>
@@ -1816,7 +2096,7 @@
       </c>
       <c r="L24" s="11"/>
       <c r="N24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
@@ -1824,28 +2104,34 @@
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
-      <c r="V24" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="8"/>
-      <c r="AA24" s="8"/>
-      <c r="AB24" s="8"/>
-    </row>
-    <row r="25" spans="6:28" ht="51.75" thickBot="1">
+      <c r="V24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="6"/>
+    </row>
+    <row r="25" spans="1:28" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F25" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="I25" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+      <c r="K25" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="L25" s="11"/>
       <c r="N25" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
@@ -1853,10 +2139,19 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
-    </row>
-    <row r="26" spans="6:28" ht="39" thickBot="1">
+      <c r="V25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+      <c r="AB25" s="8"/>
+    </row>
+    <row r="26" spans="1:28" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F26" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -1865,7 +2160,7 @@
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
       <c r="N26" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
@@ -1874,9 +2169,9 @@
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
     </row>
-    <row r="27" spans="6:28" ht="51.75" thickBot="1">
+    <row r="27" spans="1:28" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F27" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -1885,7 +2180,7 @@
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
       <c r="N27" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
@@ -1894,9 +2189,9 @@
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
     </row>
-    <row r="28" spans="6:28" ht="26.25" thickBot="1">
+    <row r="28" spans="1:28" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -1904,70 +2199,70 @@
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
       <c r="L28" s="11"/>
-    </row>
-    <row r="29" spans="6:28" ht="15.75" thickBot="1">
-      <c r="N29" s="9"/>
-      <c r="O29" s="10" t="s">
+      <c r="N28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+    </row>
+    <row r="29" spans="1:28" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+    </row>
+    <row r="30" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="9"/>
+      <c r="O30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="P29" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q29" s="10" t="s">
+      <c r="P30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q30" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="R29" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="S29" s="10" t="s">
+      <c r="R30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="S30" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="T29" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="6:28" ht="51.75" thickBot="1">
-      <c r="F30" s="5"/>
-      <c r="G30" s="5" t="s">
+      <c r="T30" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="5"/>
+      <c r="G31" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I30" s="5" t="s">
+      <c r="H31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J30" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="K30" s="5" t="s">
+      <c r="J31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L30" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="N30" s="7" t="s">
+      <c r="L31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N31" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-    </row>
-    <row r="31" spans="6:28" ht="39" thickBot="1">
-      <c r="F31" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="N31" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
@@ -1976,9 +2271,9 @@
       <c r="S31" s="11"/>
       <c r="T31" s="11"/>
     </row>
-    <row r="32" spans="6:28" ht="51.75" thickBot="1">
+    <row r="32" spans="1:28" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F32" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -1987,7 +2282,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="N32" s="7" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
@@ -1996,9 +2291,9 @@
       <c r="S32" s="11"/>
       <c r="T32" s="11"/>
     </row>
-    <row r="33" spans="6:20" ht="39" thickBot="1">
+    <row r="33" spans="6:20" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F33" s="5" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -2007,24 +2302,18 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="N33" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O33" s="11" t="s">
-        <v>26</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="O33" s="11"/>
       <c r="P33" s="11"/>
-      <c r="Q33" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="Q33" s="11"/>
       <c r="R33" s="11"/>
-      <c r="S33" s="11" t="s">
-        <v>26</v>
-      </c>
+      <c r="S33" s="11"/>
       <c r="T33" s="11"/>
     </row>
-    <row r="34" spans="6:20" ht="39" thickBot="1">
+    <row r="34" spans="6:20" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F34" s="5" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -2033,18 +2322,24 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="N34" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="O34" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="O34" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
+      <c r="Q34" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
+      <c r="S34" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="T34" s="11"/>
     </row>
-    <row r="35" spans="6:20" ht="51.75" thickBot="1">
+    <row r="35" spans="6:20" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F35" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -2053,7 +2348,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="N35" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
@@ -2062,9 +2357,18 @@
       <c r="S35" s="11"/>
       <c r="T35" s="11"/>
     </row>
-    <row r="36" spans="6:20" ht="26.25" thickBot="1">
+    <row r="36" spans="6:20" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
       <c r="N36" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
@@ -2073,6 +2377,17 @@
       <c r="S36" s="11"/>
       <c r="T36" s="11"/>
     </row>
+    <row r="37" spans="6:20" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>